<commit_message>
update of today 1.1
</commit_message>
<xml_diff>
--- a/SIEM_Evaluation_Tool.xlsx
+++ b/SIEM_Evaluation_Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Documents\GitHub\SIEM-Selection-Methodology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE0D276-9909-41DE-883D-FF7048A89C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40687F7-B5BA-478F-AF67-17DC924950F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F4D47EB6-AEA2-4FF6-B487-7D82ABF40C70}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{F4D47EB6-AEA2-4FF6-B487-7D82ABF40C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Rules" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -802,9 +803,6 @@
     <t>OpenSearch vX.Y.Z</t>
   </si>
   <si>
-    <t xml:space="preserve">It does NOT have a FOSS recognized license (OSI or FSS) (1); It does have a FOSS recognized license (OSI or FSS) (1) (5); </t>
-  </si>
-  <si>
     <t xml:space="preserve">It is NOT supported by an Open Source Foundation (1);It is supported by an Open Source Foundation (5); </t>
   </si>
   <si>
@@ -818,13 +816,16 @@
   </si>
   <si>
     <t>The project does not have a defined release timeline, or does not have any update in the last 8 months (1); the project has at least one update in the last 8 months (2); the project has a defined release timeline and has more than one release in the last 8 month (3)s; the project has a defined timeline and more than one release in the last 5 months (4); the project has a defined time line and more than on release in the last 3 months (5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It does NOT have a FOSS recognized license (OSI or FSS) (1); It does have a FOSS recognized license (OSI or FSS) (5); </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,6 +881,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1139,7 +1148,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1163,12 +1172,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1182,7 +1185,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1228,14 +1231,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,8 +1570,8 @@
   </sheetPr>
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView tabSelected="1" topLeftCell="B175" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,20 +1601,20 @@
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="20"/>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="I1" s="49"/>
+      <c r="I1" s="73"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="72" t="s">
         <v>243</v>
       </c>
-      <c r="L1" s="49"/>
+      <c r="L1" s="73"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="72" t="s">
         <v>244</v>
       </c>
-      <c r="O1" s="49"/>
+      <c r="O1" s="73"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -1665,7 +1674,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>173</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -1706,7 +1715,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="55" t="s">
         <v>174</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1747,7 +1756,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="55" t="s">
         <v>175</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -1784,7 +1793,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>176</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -1821,7 +1830,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="55" t="s">
         <v>177</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1858,7 +1867,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="55" t="s">
         <v>178</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -1895,7 +1904,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="55" t="s">
         <v>179</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -1932,7 +1941,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="55" t="s">
         <v>180</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1968,34 +1977,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="53" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
-      <c r="B12" s="50"/>
+    <row r="12" spans="1:20" s="51" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="51"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="54" t="s">
+      <c r="H12" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I12" s="52">
+      <c r="I12" s="50">
         <f>SUM(I4:I11)</f>
         <v>1</v>
       </c>
       <c r="J12" s="9"/>
-      <c r="K12" s="54" t="s">
+      <c r="K12" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="L12" s="52">
+      <c r="L12" s="50">
         <f>SUM(L4:L11)</f>
         <v>0</v>
       </c>
       <c r="M12" s="9"/>
-      <c r="N12" s="54" t="s">
+      <c r="N12" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="O12" s="52">
+      <c r="O12" s="50">
         <f>SUM(O4:O11)</f>
         <v>0</v>
       </c>
@@ -2005,7 +2014,7 @@
       <c r="T12"/>
     </row>
     <row r="13" spans="1:20" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -2022,7 +2031,7 @@
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="55" t="s">
         <v>181</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2061,7 +2070,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="55" t="s">
         <v>182</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -2100,7 +2109,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="55" t="s">
         <v>183</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -3856,7 +3865,7 @@
       </c>
     </row>
     <row r="77" spans="1:19" s="29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="60"/>
+      <c r="A77" s="58"/>
       <c r="B77" s="26" t="s">
         <v>113</v>
       </c>
@@ -6692,8 +6701,8 @@
       <c r="N175" s="14"/>
       <c r="O175" s="14"/>
     </row>
-    <row r="176" spans="1:15" s="61" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="62"/>
+    <row r="176" spans="1:15" s="59" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="60"/>
       <c r="B176" s="20"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -6754,11 +6763,11 @@
       <c r="C178" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D178" s="63"/>
+      <c r="D178" s="61"/>
       <c r="E178" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F178" s="63">
+        <v>250</v>
+      </c>
+      <c r="F178" s="61">
         <f>1/COUNTA($C$178:$C$193)</f>
         <v>6.25E-2</v>
       </c>
@@ -6782,11 +6791,11 @@
       <c r="C179" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="D179" s="63"/>
+      <c r="D179" s="61"/>
       <c r="E179" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F179" s="63">
+        <v>245</v>
+      </c>
+      <c r="F179" s="61">
         <f t="shared" ref="F179:F193" si="4">1/COUNTA($C$178:$C$193)</f>
         <v>6.25E-2</v>
       </c>
@@ -6810,11 +6819,11 @@
       <c r="C180" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D180" s="63"/>
-      <c r="E180" s="63" t="s">
-        <v>247</v>
-      </c>
-      <c r="F180" s="63">
+      <c r="D180" s="61"/>
+      <c r="E180" s="61" t="s">
+        <v>246</v>
+      </c>
+      <c r="F180" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -6838,11 +6847,11 @@
       <c r="C181" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="D181" s="63"/>
-      <c r="E181" s="63" t="s">
-        <v>248</v>
-      </c>
-      <c r="F181" s="63">
+      <c r="D181" s="61"/>
+      <c r="E181" s="61" t="s">
+        <v>247</v>
+      </c>
+      <c r="F181" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -6866,11 +6875,11 @@
       <c r="C182" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D182" s="63"/>
+      <c r="D182" s="61"/>
       <c r="E182" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F182" s="63">
+      <c r="F182" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -6894,11 +6903,11 @@
       <c r="C183" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D183" s="64" t="s">
-        <v>249</v>
-      </c>
-      <c r="E183" s="64"/>
-      <c r="F183" s="63">
+      <c r="D183" s="62" t="s">
+        <v>248</v>
+      </c>
+      <c r="E183" s="62"/>
+      <c r="F183" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -6922,9 +6931,9 @@
       <c r="C184" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D184" s="63"/>
-      <c r="E184" s="63"/>
-      <c r="F184" s="63">
+      <c r="D184" s="61"/>
+      <c r="E184" s="61"/>
+      <c r="F184" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -6948,11 +6957,11 @@
       <c r="C185" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D185" s="65"/>
-      <c r="E185" s="65" t="s">
-        <v>250</v>
-      </c>
-      <c r="F185" s="63">
+      <c r="D185" s="63"/>
+      <c r="E185" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="F185" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -6976,9 +6985,9 @@
       <c r="C186" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D186" s="66"/>
-      <c r="E186" s="66"/>
-      <c r="F186" s="63">
+      <c r="D186" s="64"/>
+      <c r="E186" s="64"/>
+      <c r="F186" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7002,9 +7011,9 @@
       <c r="C187" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D187" s="63"/>
-      <c r="E187" s="63"/>
-      <c r="F187" s="63">
+      <c r="D187" s="61"/>
+      <c r="E187" s="61"/>
+      <c r="F187" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7028,9 +7037,9 @@
       <c r="C188" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D188" s="63"/>
-      <c r="E188" s="63"/>
-      <c r="F188" s="63">
+      <c r="D188" s="61"/>
+      <c r="E188" s="61"/>
+      <c r="F188" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7054,9 +7063,9 @@
       <c r="C189" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D189" s="67"/>
-      <c r="E189" s="67"/>
-      <c r="F189" s="63">
+      <c r="D189" s="65"/>
+      <c r="E189" s="65"/>
+      <c r="F189" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7080,9 +7089,9 @@
       <c r="C190" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D190" s="63"/>
-      <c r="E190" s="63"/>
-      <c r="F190" s="63">
+      <c r="D190" s="61"/>
+      <c r="E190" s="61"/>
+      <c r="F190" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7106,9 +7115,9 @@
       <c r="C191" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D191" s="63"/>
-      <c r="E191" s="63"/>
-      <c r="F191" s="63">
+      <c r="D191" s="61"/>
+      <c r="E191" s="61"/>
+      <c r="F191" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7132,9 +7141,9 @@
       <c r="C192" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D192" s="64"/>
-      <c r="E192" s="64"/>
-      <c r="F192" s="63">
+      <c r="D192" s="62"/>
+      <c r="E192" s="62"/>
+      <c r="F192" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7158,9 +7167,9 @@
       <c r="C193" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D193" s="64"/>
-      <c r="E193" s="64"/>
-      <c r="F193" s="63">
+      <c r="D193" s="62"/>
+      <c r="E193" s="62"/>
+      <c r="F193" s="61">
         <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
@@ -7178,13 +7187,13 @@
       <c r="O193" s="14"/>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B194" s="50"/>
-      <c r="C194" s="71"/>
-      <c r="D194" s="72"/>
-      <c r="E194" s="72"/>
-      <c r="F194" s="55"/>
+      <c r="B194" s="48"/>
+      <c r="C194" s="53"/>
+      <c r="D194" s="69"/>
+      <c r="E194" s="69"/>
+      <c r="F194" s="53"/>
       <c r="G194" s="4"/>
-      <c r="H194" s="73" t="s">
+      <c r="H194" s="70" t="s">
         <v>118</v>
       </c>
       <c r="I194" s="8"/>
@@ -7195,13 +7204,13 @@
       <c r="N194" s="14"/>
       <c r="O194" s="14"/>
     </row>
-    <row r="195" spans="1:15" s="61" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="62"/>
-      <c r="B195" s="68"/>
-      <c r="C195" s="69"/>
-      <c r="D195" s="70"/>
-      <c r="E195" s="70"/>
-      <c r="F195" s="69"/>
+    <row r="195" spans="1:15" s="59" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="60"/>
+      <c r="B195" s="66"/>
+      <c r="C195" s="67"/>
+      <c r="D195" s="68"/>
+      <c r="E195" s="68"/>
+      <c r="F195" s="67"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
@@ -7257,9 +7266,9 @@
       <c r="C197" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D197" s="63"/>
-      <c r="E197" s="63"/>
-      <c r="F197" s="63"/>
+      <c r="D197" s="61"/>
+      <c r="E197" s="61"/>
+      <c r="F197" s="61"/>
       <c r="G197" s="4"/>
       <c r="H197" s="14"/>
       <c r="I197" s="14"/>
@@ -7406,7 +7415,7 @@
       <c r="B206" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C206" s="66"/>
+      <c r="C206" s="64"/>
       <c r="D206" s="30"/>
       <c r="E206" s="30"/>
       <c r="F206" s="30"/>
@@ -7424,7 +7433,7 @@
       <c r="B207" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C207" s="63"/>
+      <c r="C207" s="61"/>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
       <c r="F207" s="3"/>
@@ -7642,7 +7651,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7680,7 +7689,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -7693,7 +7702,7 @@
       <c r="D3" s="40">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="71">
         <v>0.22</v>
       </c>
     </row>
@@ -7714,7 +7723,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -7724,7 +7733,7 @@
       <c r="C5" s="40">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="71">
         <v>0.22</v>
       </c>
       <c r="E5" s="40">
@@ -7748,7 +7757,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -7758,7 +7767,7 @@
       <c r="C7" s="40">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="71">
         <v>0.22</v>
       </c>
       <c r="E7" s="40">
@@ -7782,7 +7791,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -7795,18 +7804,18 @@
       <c r="D9" s="40">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="71">
         <v>0.22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="71">
         <v>0.22</v>
       </c>
       <c r="D10" s="40">
@@ -7816,14 +7825,14 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="71">
         <v>0.22</v>
       </c>
       <c r="D11" s="40">
@@ -7861,7 +7870,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>